<commit_message>
Convert main HVAC filter from coil to system and column "object"
</commit_message>
<xml_diff>
--- a/commercial measures/SWHC046-04 Pkg HP AC Com/coil_list.xlsx
+++ b/commercial measures/SWHC046-04 Pkg HP AC Com/coil_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEER2026\dev-SWHC046-VarFan\commercial measures\SWHC046-04 Pkg HP AC Com\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DC6C60-5D96-4D28-9B6B-71F68A564EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AD5728-6677-4854-847B-254BD9A2AE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E3B3AE82-7409-46E2-9CE0-4D4F0165DBF4}"/>
+    <workbookView xWindow="-28215" yWindow="4965" windowWidth="24435" windowHeight="10200" xr2:uid="{E3B3AE82-7409-46E2-9CE0-4D4F0165DBF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Main coils" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2370" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2370" uniqueCount="392">
   <si>
     <t>BuildType</t>
   </si>
@@ -797,17 +797,479 @@
     <t>KITCHEN EL1 WEST PERIM SPC (G.W6) SZ-CAV COOLING COIL</t>
   </si>
   <si>
-    <t>cooling coil name</t>
-  </si>
-  <si>
     <t>building type</t>
+  </si>
+  <si>
+    <t>NE CORNER OFFICE SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>NW CORNER OFFICE SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>SE CORNER OFFICE SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>SW CORNER OFFICE SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CORE AUDITORIUM SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>SHOP EL1 WEST PERIM SPC (G.W1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM EL2 NORTH PERIM SPC (G.N3) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM EL2 SOUTH PERIM SPC (G.S2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM EL2 WEST PERIM SPC (G.W1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>DINING EL3 SW PERIM SPC (G.SW1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM EL4 EAST PERIM SPC (G.E2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM EL4 NORTH PERIM SPC (G.N3) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM EL4 SOUTH PERIM SPC (G.S1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM EL4 WEST PERIM SPC (G.W4) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL4 CORE SPC (G.C6) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM EL4 EAST PERIM SPC (T.E14) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM EL4 NORTH PERIM SPC (T.N15) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM EL4 SOUTH PERIM SPC (T.S13) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM EL4 WEST PERIM SPC (T.W16) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL4 CORE SPC (T.C18) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM G.E1 SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM G.NNE2 SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM G.SSE3 SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM G.W4 SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>DINING G.SSW1 SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>GYMNASIUM G.N2 SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM EL1 SPC (G.1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM E2 NORTH PERIM (G.N3) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM E2 SOUTH PERIM (G.S2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM E2 WEST PERIM (G.W1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM E4 CORE (G.C6) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM E4 EAST PERIM (G.E2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM E4 NORTH PERIM (G.N3) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM E4 SOUTH PERIM (G.S1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM E4 WEST PERIM (G.W4) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>DINING E3 SOUTH PERIM (G.S1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>MAINTENANCE E1 WEST PERIM (G.W1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE E4 CORE (G.C6) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM E4 EAST PERIM (M.E14) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM E4 NORTH PERIM (M.N15) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM E4 SOUTH PERIM (M.S13) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM E4 WEST PERIM (M.W16) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE E4 CORE (M.C18) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM E4 EAST PERIM (T.E26) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM E4 NORTH PERIM (T.N27) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM E4 SOUTH PERIM (T.S25) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CLASSROOM E4 WEST PERIM (T.W28) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE E4 CORE (T.C30) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CORRIDOR E9 CORE (G.C3) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CORRIDOR E9 CORE (M.C6) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CORRIDOR E9 CORE (T.C9) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>GROCERY SALES EL1 SSE PERIM SPC (G.SSE1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>INDLOADDOCK EL1 NORTH PERIM SPC (G.N3) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL1 SW PERIM SPC (G.SW2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>REFFOODPREP EL1 CORE SPC (G.C4) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>REFWALKINCOOL EL1 CORE SPC (G.C6) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>REFWALKINFREEZE EL1 CORE SPC (G.C5) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>DINING EL1 NORTH PERIM (G.N1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>DINING EL1 SOUTH PERIM (G.S2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL2 CORE (G.C7) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL2 EAST PERIM (G.E1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL2 NORTH PERIM (G.N6) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL2 SOUTH PERIM (G.S5) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>SURGERY EL2 NNW PERIM (G.NNW3) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>SURGERY EL2 SSW PERIM (G.SSW2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>SURGERY EL2 WEST PERIM (G.W4) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>BARCASINO EL2 NORTH PERIM SPC (G.N2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>BARCASINO EL3 NORTH PERIM SPC (G.N1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CORRIDOR EL4 CORE SPC (G.C5) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CORRIDOR EL4 CORE SPC (M.C15) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CORRIDOR EL4 CORE SPC (T.C25) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>DINING EL2 WEST PERIM SPC (G.W3) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>DINING EL3 WEST PERIM SPC (G.W3) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>LAUNDRY EL1 WEST PERIM SPC (G.W1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>LOBBY EL1 WEST PERIM SPC (G.W2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL1 EAST PERIM SPC (G.E3) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CONFERENCE EL1 CORE SPC (G.C7) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CORRIDOR EL1 CORE SPC (G.C6) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>DINING EL1 CORE SPC (G.C9) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL1 CORE SPC (G.C11) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL1 EAST PERIM SPC (G.E2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL1 NORTH PERIM SPC (G.N3) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL1 SOUTH PERIM SPC (G.S1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL1 WEST PERIM SPC (G.W4) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>STOCKROOM EL1 NE PERIM SPC (G.NE2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>STOCKROOM EL1 SW PERIM SPC (G.SW3) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>WORK EL1 SOUTH PERIM SPC (G.S1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CORRIDOR EL1 CORE PERIM SPC (G.C5) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CORRIDOR EL1 SOUTH PERIM SPC (G.S9) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CORRIDOR EL2 CORE SPC (G.C5) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CORRIDOR EL2 NNE PERIM SPC (G.NNE4) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CORRIDOR EL2 NORTH PERIM SPC (G.N1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CORRIDOR EL2 NORTH PERIM SPC (G.N3) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CORRIDOR EL2 SSW PERIM SPC (G.SSW2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CORRIDOR EL2 SOUTH PERIM SPC (G.S6) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>CORRIDOR EL2 SOUTH PERIM SPC (G.S7) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>LAUNDRY EL1 SOUTH PERIM SPC (G.S7) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL1 SE PERIM SPC (G.SE6) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>DINING EL1 WEST PERIM SPC (G.W1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL2 CORE SPC (G.C1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL2 NORTH PERIM SPC (G.N3) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL2 SOUTH PERIM SPC (G.S2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL3 NORTH PERIM SPC (G.N3) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL3 SOUTH PERIM SPC (G.S2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL3 WEST PERIM SPC (G.W1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICEOPEN EL1 CORE SPC (M.C15) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICEOPEN EL1 CORE SPC (T.C25) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICESMALL EL1 EAST PERIM SPC (M.E12) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICESMALL EL1 EAST PERIM SPC (T.E22) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICESMALL EL1 NORTH PERIM SPC (M.N13) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICESMALL EL1 NORTH PERIM SPC (T.N23) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICESMALL EL1 SOUTH PERIM SPC (M.S11) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICESMALL EL1 SOUTH PERIM SPC (T.S21) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICESMALL EL1 WEST PERIM SPC (M.W14) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICESMALL EL1 WEST PERIM SPC (T.W24) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>HALL EL1 CORE SPC (G.C5) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICESMALL EL1 NORTH PERIM SPC (G.N3) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICESMALL EL1 EAST PERIM SPC (G.E2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICESMALL EL1 SOUTH PERIM SPC (G.S1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICESMALL EL1 WEST PERIM SPC (G.W4) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>HALL EL1 CORE SPC (T.C15) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICESMALL EL1 EAST PERIM SPC (T.E12) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICESMALL EL1 NORTH PERIM SPC (T.N13) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICESMALL EL1 SOUTH PERIM SPC (T.S11) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICESMALL EL1 WEST PERIM SPC (T.W14) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>DINING EL1 ESE PERIM SPC (G.ESE1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>LOBBYWAITING EL1 SSW PERIM SPC (G.SSW2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>RESTROOM EL1 NORTH PERIM SPC (G.N4) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>LOBBYWAITING EL1 SW PERIM SPC (G.SW2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>EL1 CORE SPC (G.C5) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>RETAILSALES EL1 NORTH PERIM SPC (G.N3) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>RETAILSALES EL1 SOUTH PERIM SPC (G.S1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>RETAILSALES EL1 WEST PERIM SPC (G.W4) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>RETAILSALES EL1 CORE SPC (M.C15) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>RETAILSALES EL1 EAST PERIM SPC (M.E12) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>RETAILSALES EL1 NORTH PERIM SPC (M.N13) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>RETAILSALES EL1 SOUTH PERIM SPC (M.S11) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>RETAILSALES EL1 WEST PERIM SPC (M.W14) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>RETAILSALES EL1 CORE SPC (T.C25) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>RETAILSALES EL1 EAST PERIM SPC (T.E22) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>RETAILSALES EL1 NORTH PERIM SPC (T.N23) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>RETAILSALES EL1 SOUTH PERIM SPC (T.S21) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>RETAILSALES EL1 WEST PERIM SPC (T.W24) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>AUTOSHOP EL1 WEST PERIM SPC (G.W5) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>OFFICE EL1 EAST PERIM SPC (G.E4) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>RETAIL EL1 CORE SPC (G.C8) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>RETAIL EL1 SOUTH PERIM SPC (G.S1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>RETAIL EL1 WSW PERIM SPC (G.WSW7) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>STOCK EL1 EAST PERIM SPC (G.E3) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>STOCK EL1 NORTH PERIM SPC (G.N2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>RETAILSALES EL1 SOUTH PERIM (G.S1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>STOCKROOM EL1 NORTH PERIM (G.N2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>WAREHOUSECOND EL1 NORTH PERIM SPC (G.N2) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>WAREHOUSECOND EL1 SOUTH PERIM SPC (G.S1) SZ-CAV UNITARY</t>
+  </si>
+  <si>
+    <t>object name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -828,12 +1290,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1225,7 +1681,7 @@
   <dimension ref="A1:E163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,10 +1699,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>236</v>
+        <v>391</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
@@ -1263,7 +1719,7 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>237</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -1281,7 +1737,7 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>238</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -1299,7 +1755,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>239</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -1317,7 +1773,7 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>240</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -1335,7 +1791,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>241</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -1353,7 +1809,7 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>242</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -1371,7 +1827,7 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>243</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -1389,7 +1845,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>244</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
@@ -1407,7 +1863,7 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>245</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
@@ -1425,7 +1881,7 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>246</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
@@ -1443,7 +1899,7 @@
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>247</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -1461,7 +1917,7 @@
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>248</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -1479,7 +1935,7 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>249</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -1497,7 +1953,7 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>250</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -1515,7 +1971,7 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>251</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
@@ -1533,7 +1989,7 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>252</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
@@ -1551,7 +2007,7 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>253</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
@@ -1569,7 +2025,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>254</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
@@ -1587,7 +2043,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>255</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
@@ -1605,7 +2061,7 @@
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>256</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
@@ -1623,7 +2079,7 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>257</v>
       </c>
       <c r="D22" t="s">
         <v>5</v>
@@ -1641,7 +2097,7 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>258</v>
       </c>
       <c r="D23" t="s">
         <v>5</v>
@@ -1659,7 +2115,7 @@
         <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>259</v>
       </c>
       <c r="D24" t="s">
         <v>5</v>
@@ -1677,7 +2133,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>260</v>
       </c>
       <c r="D25" t="s">
         <v>5</v>
@@ -1695,7 +2151,7 @@
         <v>19</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>261</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
@@ -1713,7 +2169,7 @@
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>64</v>
+        <v>262</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
@@ -1731,7 +2187,7 @@
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>263</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
@@ -1749,7 +2205,7 @@
         <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>264</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
@@ -1767,7 +2223,7 @@
         <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>265</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
@@ -1785,7 +2241,7 @@
         <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>266</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
@@ -1803,7 +2259,7 @@
         <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>267</v>
       </c>
       <c r="D32" t="s">
         <v>5</v>
@@ -1821,7 +2277,7 @@
         <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>268</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>
@@ -1839,7 +2295,7 @@
         <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
+        <v>269</v>
       </c>
       <c r="D34" t="s">
         <v>5</v>
@@ -1857,7 +2313,7 @@
         <v>21</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>270</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
@@ -1875,7 +2331,7 @@
         <v>21</v>
       </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>271</v>
       </c>
       <c r="D36" t="s">
         <v>5</v>
@@ -1893,7 +2349,7 @@
         <v>22</v>
       </c>
       <c r="C37" t="s">
-        <v>66</v>
+        <v>264</v>
       </c>
       <c r="D37" t="s">
         <v>5</v>
@@ -1911,7 +2367,7 @@
         <v>22</v>
       </c>
       <c r="C38" t="s">
-        <v>67</v>
+        <v>265</v>
       </c>
       <c r="D38" t="s">
         <v>5</v>
@@ -1929,7 +2385,7 @@
         <v>22</v>
       </c>
       <c r="C39" t="s">
-        <v>68</v>
+        <v>266</v>
       </c>
       <c r="D39" t="s">
         <v>5</v>
@@ -1947,7 +2403,7 @@
         <v>22</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>272</v>
       </c>
       <c r="D40" t="s">
         <v>5</v>
@@ -1965,7 +2421,7 @@
         <v>22</v>
       </c>
       <c r="C41" t="s">
-        <v>75</v>
+        <v>273</v>
       </c>
       <c r="D41" t="s">
         <v>5</v>
@@ -1983,7 +2439,7 @@
         <v>22</v>
       </c>
       <c r="C42" t="s">
-        <v>70</v>
+        <v>268</v>
       </c>
       <c r="D42" t="s">
         <v>5</v>
@@ -2001,7 +2457,7 @@
         <v>22</v>
       </c>
       <c r="C43" t="s">
-        <v>71</v>
+        <v>269</v>
       </c>
       <c r="D43" t="s">
         <v>5</v>
@@ -2019,7 +2475,7 @@
         <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>72</v>
+        <v>270</v>
       </c>
       <c r="D44" t="s">
         <v>5</v>
@@ -2037,7 +2493,7 @@
         <v>22</v>
       </c>
       <c r="C45" t="s">
-        <v>73</v>
+        <v>271</v>
       </c>
       <c r="D45" t="s">
         <v>5</v>
@@ -2055,7 +2511,7 @@
         <v>22</v>
       </c>
       <c r="C46" t="s">
-        <v>76</v>
+        <v>274</v>
       </c>
       <c r="D46" t="s">
         <v>5</v>
@@ -2073,7 +2529,7 @@
         <v>22</v>
       </c>
       <c r="C47" t="s">
-        <v>77</v>
+        <v>275</v>
       </c>
       <c r="D47" t="s">
         <v>5</v>
@@ -2091,7 +2547,7 @@
         <v>22</v>
       </c>
       <c r="C48" t="s">
-        <v>78</v>
+        <v>276</v>
       </c>
       <c r="D48" t="s">
         <v>5</v>
@@ -2109,7 +2565,7 @@
         <v>22</v>
       </c>
       <c r="C49" t="s">
-        <v>79</v>
+        <v>277</v>
       </c>
       <c r="D49" t="s">
         <v>5</v>
@@ -2127,7 +2583,7 @@
         <v>22</v>
       </c>
       <c r="C50" t="s">
-        <v>80</v>
+        <v>278</v>
       </c>
       <c r="D50" t="s">
         <v>5</v>
@@ -2145,7 +2601,7 @@
         <v>22</v>
       </c>
       <c r="C51" t="s">
-        <v>81</v>
+        <v>279</v>
       </c>
       <c r="D51" t="s">
         <v>5</v>
@@ -2163,7 +2619,7 @@
         <v>22</v>
       </c>
       <c r="C52" t="s">
-        <v>82</v>
+        <v>280</v>
       </c>
       <c r="D52" t="s">
         <v>5</v>
@@ -2181,7 +2637,7 @@
         <v>22</v>
       </c>
       <c r="C53" t="s">
-        <v>83</v>
+        <v>281</v>
       </c>
       <c r="D53" t="s">
         <v>5</v>
@@ -2199,7 +2655,7 @@
         <v>22</v>
       </c>
       <c r="C54" t="s">
-        <v>84</v>
+        <v>282</v>
       </c>
       <c r="D54" t="s">
         <v>5</v>
@@ -2217,7 +2673,7 @@
         <v>22</v>
       </c>
       <c r="C55" t="s">
-        <v>85</v>
+        <v>283</v>
       </c>
       <c r="D55" t="s">
         <v>5</v>
@@ -2235,7 +2691,7 @@
         <v>22</v>
       </c>
       <c r="C56" t="s">
-        <v>86</v>
+        <v>284</v>
       </c>
       <c r="D56" t="s">
         <v>5</v>
@@ -2253,7 +2709,7 @@
         <v>22</v>
       </c>
       <c r="C57" t="s">
-        <v>87</v>
+        <v>285</v>
       </c>
       <c r="D57" t="s">
         <v>5</v>
@@ -2271,7 +2727,7 @@
         <v>22</v>
       </c>
       <c r="C58" t="s">
-        <v>88</v>
+        <v>286</v>
       </c>
       <c r="D58" t="s">
         <v>5</v>
@@ -2289,7 +2745,7 @@
         <v>22</v>
       </c>
       <c r="C59" t="s">
-        <v>89</v>
+        <v>287</v>
       </c>
       <c r="D59" t="s">
         <v>5</v>
@@ -2307,7 +2763,7 @@
         <v>23</v>
       </c>
       <c r="C60" t="s">
-        <v>90</v>
+        <v>288</v>
       </c>
       <c r="D60" t="s">
         <v>5</v>
@@ -2325,7 +2781,7 @@
         <v>23</v>
       </c>
       <c r="C61" t="s">
-        <v>91</v>
+        <v>289</v>
       </c>
       <c r="D61" t="s">
         <v>5</v>
@@ -2343,7 +2799,7 @@
         <v>23</v>
       </c>
       <c r="C62" t="s">
-        <v>92</v>
+        <v>290</v>
       </c>
       <c r="D62" t="s">
         <v>5</v>
@@ -2361,7 +2817,7 @@
         <v>23</v>
       </c>
       <c r="C63" t="s">
-        <v>93</v>
+        <v>291</v>
       </c>
       <c r="D63" t="s">
         <v>5</v>
@@ -2379,7 +2835,7 @@
         <v>23</v>
       </c>
       <c r="C64" t="s">
-        <v>94</v>
+        <v>292</v>
       </c>
       <c r="D64" t="s">
         <v>5</v>
@@ -2397,7 +2853,7 @@
         <v>23</v>
       </c>
       <c r="C65" t="s">
-        <v>95</v>
+        <v>293</v>
       </c>
       <c r="D65" t="s">
         <v>5</v>
@@ -2415,7 +2871,7 @@
         <v>24</v>
       </c>
       <c r="C66" t="s">
-        <v>96</v>
+        <v>294</v>
       </c>
       <c r="D66" t="s">
         <v>5</v>
@@ -2433,7 +2889,7 @@
         <v>24</v>
       </c>
       <c r="C67" t="s">
-        <v>97</v>
+        <v>295</v>
       </c>
       <c r="D67" t="s">
         <v>5</v>
@@ -2451,7 +2907,7 @@
         <v>24</v>
       </c>
       <c r="C68" t="s">
-        <v>98</v>
+        <v>296</v>
       </c>
       <c r="D68" t="s">
         <v>5</v>
@@ -2469,7 +2925,7 @@
         <v>24</v>
       </c>
       <c r="C69" t="s">
-        <v>99</v>
+        <v>297</v>
       </c>
       <c r="D69" t="s">
         <v>5</v>
@@ -2487,7 +2943,7 @@
         <v>24</v>
       </c>
       <c r="C70" t="s">
-        <v>100</v>
+        <v>298</v>
       </c>
       <c r="D70" t="s">
         <v>5</v>
@@ -2505,7 +2961,7 @@
         <v>24</v>
       </c>
       <c r="C71" t="s">
-        <v>101</v>
+        <v>299</v>
       </c>
       <c r="D71" t="s">
         <v>5</v>
@@ -2523,7 +2979,7 @@
         <v>24</v>
       </c>
       <c r="C72" t="s">
-        <v>102</v>
+        <v>300</v>
       </c>
       <c r="D72" t="s">
         <v>5</v>
@@ -2541,7 +2997,7 @@
         <v>24</v>
       </c>
       <c r="C73" t="s">
-        <v>103</v>
+        <v>301</v>
       </c>
       <c r="D73" t="s">
         <v>5</v>
@@ -2559,7 +3015,7 @@
         <v>24</v>
       </c>
       <c r="C74" t="s">
-        <v>104</v>
+        <v>302</v>
       </c>
       <c r="D74" t="s">
         <v>5</v>
@@ -2577,7 +3033,7 @@
         <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>7</v>
+        <v>303</v>
       </c>
       <c r="D75" t="s">
         <v>5</v>
@@ -2595,7 +3051,7 @@
         <v>3</v>
       </c>
       <c r="C76" t="s">
-        <v>8</v>
+        <v>304</v>
       </c>
       <c r="D76" t="s">
         <v>5</v>
@@ -2613,7 +3069,7 @@
         <v>3</v>
       </c>
       <c r="C77" t="s">
-        <v>9</v>
+        <v>305</v>
       </c>
       <c r="D77" t="s">
         <v>5</v>
@@ -2631,7 +3087,7 @@
         <v>3</v>
       </c>
       <c r="C78" t="s">
-        <v>10</v>
+        <v>306</v>
       </c>
       <c r="D78" t="s">
         <v>5</v>
@@ -2649,7 +3105,7 @@
         <v>3</v>
       </c>
       <c r="C79" t="s">
-        <v>11</v>
+        <v>307</v>
       </c>
       <c r="D79" t="s">
         <v>5</v>
@@ -2667,7 +3123,7 @@
         <v>3</v>
       </c>
       <c r="C80" t="s">
-        <v>12</v>
+        <v>308</v>
       </c>
       <c r="D80" t="s">
         <v>5</v>
@@ -2685,7 +3141,7 @@
         <v>3</v>
       </c>
       <c r="C81" t="s">
-        <v>13</v>
+        <v>309</v>
       </c>
       <c r="D81" t="s">
         <v>5</v>
@@ -2703,7 +3159,7 @@
         <v>3</v>
       </c>
       <c r="C82" t="s">
-        <v>14</v>
+        <v>310</v>
       </c>
       <c r="D82" t="s">
         <v>5</v>
@@ -2721,7 +3177,7 @@
         <v>3</v>
       </c>
       <c r="C83" t="s">
-        <v>15</v>
+        <v>311</v>
       </c>
       <c r="D83" t="s">
         <v>5</v>
@@ -2739,7 +3195,7 @@
         <v>3</v>
       </c>
       <c r="C84" t="s">
-        <v>16</v>
+        <v>312</v>
       </c>
       <c r="D84" t="s">
         <v>5</v>
@@ -2757,7 +3213,7 @@
         <v>25</v>
       </c>
       <c r="C85" t="s">
-        <v>105</v>
+        <v>313</v>
       </c>
       <c r="D85" t="s">
         <v>5</v>
@@ -2775,7 +3231,7 @@
         <v>25</v>
       </c>
       <c r="C86" t="s">
-        <v>106</v>
+        <v>314</v>
       </c>
       <c r="D86" t="s">
         <v>5</v>
@@ -2793,7 +3249,7 @@
         <v>25</v>
       </c>
       <c r="C87" t="s">
-        <v>107</v>
+        <v>315</v>
       </c>
       <c r="D87" t="s">
         <v>5</v>
@@ -2811,7 +3267,7 @@
         <v>25</v>
       </c>
       <c r="C88" t="s">
-        <v>108</v>
+        <v>316</v>
       </c>
       <c r="D88" t="s">
         <v>5</v>
@@ -2829,7 +3285,7 @@
         <v>25</v>
       </c>
       <c r="C89" t="s">
-        <v>109</v>
+        <v>317</v>
       </c>
       <c r="D89" t="s">
         <v>5</v>
@@ -2847,7 +3303,7 @@
         <v>25</v>
       </c>
       <c r="C90" t="s">
-        <v>110</v>
+        <v>318</v>
       </c>
       <c r="D90" t="s">
         <v>5</v>
@@ -2865,7 +3321,7 @@
         <v>25</v>
       </c>
       <c r="C91" t="s">
-        <v>111</v>
+        <v>319</v>
       </c>
       <c r="D91" t="s">
         <v>5</v>
@@ -2883,7 +3339,7 @@
         <v>25</v>
       </c>
       <c r="C92" t="s">
-        <v>112</v>
+        <v>320</v>
       </c>
       <c r="D92" t="s">
         <v>5</v>
@@ -2901,7 +3357,7 @@
         <v>26</v>
       </c>
       <c r="C93" t="s">
-        <v>113</v>
+        <v>321</v>
       </c>
       <c r="D93" t="s">
         <v>5</v>
@@ -2919,7 +3375,7 @@
         <v>26</v>
       </c>
       <c r="C94" t="s">
-        <v>114</v>
+        <v>322</v>
       </c>
       <c r="D94" t="s">
         <v>5</v>
@@ -2937,7 +3393,7 @@
         <v>26</v>
       </c>
       <c r="C95" t="s">
-        <v>115</v>
+        <v>323</v>
       </c>
       <c r="D95" t="s">
         <v>5</v>
@@ -2955,7 +3411,7 @@
         <v>27</v>
       </c>
       <c r="C96" t="s">
-        <v>116</v>
+        <v>324</v>
       </c>
       <c r="D96" t="s">
         <v>5</v>
@@ -2973,7 +3429,7 @@
         <v>27</v>
       </c>
       <c r="C97" t="s">
-        <v>117</v>
+        <v>325</v>
       </c>
       <c r="D97" t="s">
         <v>5</v>
@@ -2991,7 +3447,7 @@
         <v>27</v>
       </c>
       <c r="C98" t="s">
-        <v>118</v>
+        <v>326</v>
       </c>
       <c r="D98" t="s">
         <v>5</v>
@@ -3009,7 +3465,7 @@
         <v>27</v>
       </c>
       <c r="C99" t="s">
-        <v>119</v>
+        <v>327</v>
       </c>
       <c r="D99" t="s">
         <v>5</v>
@@ -3027,7 +3483,7 @@
         <v>27</v>
       </c>
       <c r="C100" t="s">
-        <v>120</v>
+        <v>328</v>
       </c>
       <c r="D100" t="s">
         <v>5</v>
@@ -3045,7 +3501,7 @@
         <v>27</v>
       </c>
       <c r="C101" t="s">
-        <v>121</v>
+        <v>329</v>
       </c>
       <c r="D101" t="s">
         <v>5</v>
@@ -3063,7 +3519,7 @@
         <v>27</v>
       </c>
       <c r="C102" t="s">
-        <v>122</v>
+        <v>330</v>
       </c>
       <c r="D102" t="s">
         <v>5</v>
@@ -3081,7 +3537,7 @@
         <v>27</v>
       </c>
       <c r="C103" t="s">
-        <v>123</v>
+        <v>331</v>
       </c>
       <c r="D103" t="s">
         <v>5</v>
@@ -3099,7 +3555,7 @@
         <v>27</v>
       </c>
       <c r="C104" t="s">
-        <v>124</v>
+        <v>332</v>
       </c>
       <c r="D104" t="s">
         <v>5</v>
@@ -3117,7 +3573,7 @@
         <v>27</v>
       </c>
       <c r="C105" t="s">
-        <v>125</v>
+        <v>333</v>
       </c>
       <c r="D105" t="s">
         <v>5</v>
@@ -3135,7 +3591,7 @@
         <v>27</v>
       </c>
       <c r="C106" t="s">
-        <v>126</v>
+        <v>334</v>
       </c>
       <c r="D106" t="s">
         <v>5</v>
@@ -3153,7 +3609,7 @@
         <v>28</v>
       </c>
       <c r="C107" t="s">
-        <v>127</v>
+        <v>335</v>
       </c>
       <c r="D107" t="s">
         <v>5</v>
@@ -3171,7 +3627,7 @@
         <v>28</v>
       </c>
       <c r="C108" t="s">
-        <v>128</v>
+        <v>336</v>
       </c>
       <c r="D108" t="s">
         <v>5</v>
@@ -3189,7 +3645,7 @@
         <v>28</v>
       </c>
       <c r="C109" t="s">
-        <v>129</v>
+        <v>337</v>
       </c>
       <c r="D109" t="s">
         <v>5</v>
@@ -3207,7 +3663,7 @@
         <v>28</v>
       </c>
       <c r="C110" t="s">
-        <v>130</v>
+        <v>338</v>
       </c>
       <c r="D110" t="s">
         <v>5</v>
@@ -3225,7 +3681,7 @@
         <v>28</v>
       </c>
       <c r="C111" t="s">
-        <v>131</v>
+        <v>339</v>
       </c>
       <c r="D111" t="s">
         <v>5</v>
@@ -3243,7 +3699,7 @@
         <v>28</v>
       </c>
       <c r="C112" t="s">
-        <v>132</v>
+        <v>340</v>
       </c>
       <c r="D112" t="s">
         <v>5</v>
@@ -3261,7 +3717,7 @@
         <v>28</v>
       </c>
       <c r="C113" t="s">
-        <v>133</v>
+        <v>341</v>
       </c>
       <c r="D113" t="s">
         <v>5</v>
@@ -3279,7 +3735,7 @@
         <v>29</v>
       </c>
       <c r="C114" t="s">
-        <v>134</v>
+        <v>342</v>
       </c>
       <c r="D114" t="s">
         <v>5</v>
@@ -3297,7 +3753,7 @@
         <v>29</v>
       </c>
       <c r="C115" t="s">
-        <v>135</v>
+        <v>343</v>
       </c>
       <c r="D115" t="s">
         <v>5</v>
@@ -3315,7 +3771,7 @@
         <v>29</v>
       </c>
       <c r="C116" t="s">
-        <v>136</v>
+        <v>344</v>
       </c>
       <c r="D116" t="s">
         <v>5</v>
@@ -3333,7 +3789,7 @@
         <v>29</v>
       </c>
       <c r="C117" t="s">
-        <v>137</v>
+        <v>345</v>
       </c>
       <c r="D117" t="s">
         <v>5</v>
@@ -3351,7 +3807,7 @@
         <v>29</v>
       </c>
       <c r="C118" t="s">
-        <v>138</v>
+        <v>346</v>
       </c>
       <c r="D118" t="s">
         <v>5</v>
@@ -3369,7 +3825,7 @@
         <v>29</v>
       </c>
       <c r="C119" t="s">
-        <v>139</v>
+        <v>347</v>
       </c>
       <c r="D119" t="s">
         <v>5</v>
@@ -3387,7 +3843,7 @@
         <v>29</v>
       </c>
       <c r="C120" t="s">
-        <v>140</v>
+        <v>348</v>
       </c>
       <c r="D120" t="s">
         <v>5</v>
@@ -3405,7 +3861,7 @@
         <v>29</v>
       </c>
       <c r="C121" t="s">
-        <v>141</v>
+        <v>349</v>
       </c>
       <c r="D121" t="s">
         <v>5</v>
@@ -3423,7 +3879,7 @@
         <v>29</v>
       </c>
       <c r="C122" t="s">
-        <v>142</v>
+        <v>350</v>
       </c>
       <c r="D122" t="s">
         <v>5</v>
@@ -3441,7 +3897,7 @@
         <v>29</v>
       </c>
       <c r="C123" t="s">
-        <v>143</v>
+        <v>351</v>
       </c>
       <c r="D123" t="s">
         <v>5</v>
@@ -3459,7 +3915,7 @@
         <v>30</v>
       </c>
       <c r="C124" t="s">
-        <v>144</v>
+        <v>352</v>
       </c>
       <c r="D124" t="s">
         <v>5</v>
@@ -3477,7 +3933,7 @@
         <v>30</v>
       </c>
       <c r="C125" t="s">
-        <v>145</v>
+        <v>353</v>
       </c>
       <c r="D125" t="s">
         <v>5</v>
@@ -3495,7 +3951,7 @@
         <v>30</v>
       </c>
       <c r="C126" t="s">
-        <v>146</v>
+        <v>354</v>
       </c>
       <c r="D126" t="s">
         <v>5</v>
@@ -3513,7 +3969,7 @@
         <v>30</v>
       </c>
       <c r="C127" t="s">
-        <v>147</v>
+        <v>355</v>
       </c>
       <c r="D127" t="s">
         <v>5</v>
@@ -3531,7 +3987,7 @@
         <v>30</v>
       </c>
       <c r="C128" t="s">
-        <v>148</v>
+        <v>356</v>
       </c>
       <c r="D128" t="s">
         <v>5</v>
@@ -3549,7 +4005,7 @@
         <v>30</v>
       </c>
       <c r="C129" t="s">
-        <v>149</v>
+        <v>357</v>
       </c>
       <c r="D129" t="s">
         <v>5</v>
@@ -3567,7 +4023,7 @@
         <v>30</v>
       </c>
       <c r="C130" t="s">
-        <v>150</v>
+        <v>358</v>
       </c>
       <c r="D130" t="s">
         <v>5</v>
@@ -3585,7 +4041,7 @@
         <v>30</v>
       </c>
       <c r="C131" t="s">
-        <v>151</v>
+        <v>359</v>
       </c>
       <c r="D131" t="s">
         <v>5</v>
@@ -3603,7 +4059,7 @@
         <v>30</v>
       </c>
       <c r="C132" t="s">
-        <v>152</v>
+        <v>360</v>
       </c>
       <c r="D132" t="s">
         <v>5</v>
@@ -3621,7 +4077,7 @@
         <v>30</v>
       </c>
       <c r="C133" t="s">
-        <v>153</v>
+        <v>361</v>
       </c>
       <c r="D133" t="s">
         <v>5</v>
@@ -3639,7 +4095,7 @@
         <v>31</v>
       </c>
       <c r="C134" t="s">
-        <v>154</v>
+        <v>362</v>
       </c>
       <c r="D134" t="s">
         <v>5</v>
@@ -3657,7 +4113,7 @@
         <v>31</v>
       </c>
       <c r="C135" t="s">
-        <v>155</v>
+        <v>363</v>
       </c>
       <c r="D135" t="s">
         <v>5</v>
@@ -3675,7 +4131,7 @@
         <v>31</v>
       </c>
       <c r="C136" t="s">
-        <v>34</v>
+        <v>364</v>
       </c>
       <c r="D136" t="s">
         <v>5</v>
@@ -3693,7 +4149,7 @@
         <v>32</v>
       </c>
       <c r="C137" t="s">
-        <v>33</v>
+        <v>365</v>
       </c>
       <c r="D137" t="s">
         <v>5</v>
@@ -3711,7 +4167,7 @@
         <v>32</v>
       </c>
       <c r="C138" t="s">
-        <v>34</v>
+        <v>364</v>
       </c>
       <c r="D138" t="s">
         <v>5</v>
@@ -3729,7 +4185,7 @@
         <v>35</v>
       </c>
       <c r="C139" t="s">
-        <v>156</v>
+        <v>366</v>
       </c>
       <c r="D139" t="s">
         <v>5</v>
@@ -3747,7 +4203,7 @@
         <v>35</v>
       </c>
       <c r="C140" t="s">
-        <v>157</v>
+        <v>367</v>
       </c>
       <c r="D140" t="s">
         <v>5</v>
@@ -3765,7 +4221,7 @@
         <v>35</v>
       </c>
       <c r="C141" t="s">
-        <v>158</v>
+        <v>368</v>
       </c>
       <c r="D141" t="s">
         <v>5</v>
@@ -3783,7 +4239,7 @@
         <v>35</v>
       </c>
       <c r="C142" t="s">
-        <v>159</v>
+        <v>369</v>
       </c>
       <c r="D142" t="s">
         <v>5</v>
@@ -3801,7 +4257,7 @@
         <v>35</v>
       </c>
       <c r="C143" t="s">
-        <v>160</v>
+        <v>370</v>
       </c>
       <c r="D143" t="s">
         <v>5</v>
@@ -3819,7 +4275,7 @@
         <v>35</v>
       </c>
       <c r="C144" t="s">
-        <v>161</v>
+        <v>371</v>
       </c>
       <c r="D144" t="s">
         <v>5</v>
@@ -3837,7 +4293,7 @@
         <v>35</v>
       </c>
       <c r="C145" t="s">
-        <v>162</v>
+        <v>372</v>
       </c>
       <c r="D145" t="s">
         <v>5</v>
@@ -3855,7 +4311,7 @@
         <v>35</v>
       </c>
       <c r="C146" t="s">
-        <v>163</v>
+        <v>373</v>
       </c>
       <c r="D146" t="s">
         <v>5</v>
@@ -3873,7 +4329,7 @@
         <v>35</v>
       </c>
       <c r="C147" t="s">
-        <v>164</v>
+        <v>374</v>
       </c>
       <c r="D147" t="s">
         <v>5</v>
@@ -3891,7 +4347,7 @@
         <v>35</v>
       </c>
       <c r="C148" t="s">
-        <v>165</v>
+        <v>375</v>
       </c>
       <c r="D148" t="s">
         <v>5</v>
@@ -3909,7 +4365,7 @@
         <v>35</v>
       </c>
       <c r="C149" t="s">
-        <v>166</v>
+        <v>376</v>
       </c>
       <c r="D149" t="s">
         <v>5</v>
@@ -3927,7 +4383,7 @@
         <v>35</v>
       </c>
       <c r="C150" t="s">
-        <v>167</v>
+        <v>377</v>
       </c>
       <c r="D150" t="s">
         <v>5</v>
@@ -3945,7 +4401,7 @@
         <v>35</v>
       </c>
       <c r="C151" t="s">
-        <v>168</v>
+        <v>378</v>
       </c>
       <c r="D151" t="s">
         <v>5</v>
@@ -3963,7 +4419,7 @@
         <v>35</v>
       </c>
       <c r="C152" t="s">
-        <v>169</v>
+        <v>379</v>
       </c>
       <c r="D152" t="s">
         <v>5</v>
@@ -3981,7 +4437,7 @@
         <v>36</v>
       </c>
       <c r="C153" t="s">
-        <v>170</v>
+        <v>380</v>
       </c>
       <c r="D153" t="s">
         <v>5</v>
@@ -3999,7 +4455,7 @@
         <v>36</v>
       </c>
       <c r="C154" t="s">
-        <v>171</v>
+        <v>381</v>
       </c>
       <c r="D154" t="s">
         <v>5</v>
@@ -4017,7 +4473,7 @@
         <v>36</v>
       </c>
       <c r="C155" t="s">
-        <v>172</v>
+        <v>382</v>
       </c>
       <c r="D155" t="s">
         <v>5</v>
@@ -4035,7 +4491,7 @@
         <v>36</v>
       </c>
       <c r="C156" t="s">
-        <v>173</v>
+        <v>383</v>
       </c>
       <c r="D156" t="s">
         <v>5</v>
@@ -4053,7 +4509,7 @@
         <v>36</v>
       </c>
       <c r="C157" t="s">
-        <v>174</v>
+        <v>384</v>
       </c>
       <c r="D157" t="s">
         <v>5</v>
@@ -4071,7 +4527,7 @@
         <v>36</v>
       </c>
       <c r="C158" t="s">
-        <v>175</v>
+        <v>385</v>
       </c>
       <c r="D158" t="s">
         <v>5</v>
@@ -4089,7 +4545,7 @@
         <v>36</v>
       </c>
       <c r="C159" t="s">
-        <v>176</v>
+        <v>386</v>
       </c>
       <c r="D159" t="s">
         <v>5</v>
@@ -4107,7 +4563,7 @@
         <v>37</v>
       </c>
       <c r="C160" t="s">
-        <v>177</v>
+        <v>387</v>
       </c>
       <c r="D160" t="s">
         <v>5</v>
@@ -4125,7 +4581,7 @@
         <v>37</v>
       </c>
       <c r="C161" t="s">
-        <v>178</v>
+        <v>388</v>
       </c>
       <c r="D161" t="s">
         <v>5</v>
@@ -4143,7 +4599,7 @@
         <v>38</v>
       </c>
       <c r="C162" t="s">
-        <v>179</v>
+        <v>389</v>
       </c>
       <c r="D162" t="s">
         <v>5</v>
@@ -4161,7 +4617,7 @@
         <v>38</v>
       </c>
       <c r="C163" t="s">
-        <v>180</v>
+        <v>390</v>
       </c>
       <c r="D163" t="s">
         <v>5</v>
@@ -11924,6 +12380,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="977ed3b4-dc53-4ccd-91b7-93b67a0eba97">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="63e8c1f7-1787-49b1-80e5-dcc3ae9ab6e9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100366A9EB7EB4E4F489A4515111482199D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="db4c11ca1524f4dab84562af922705c9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="977ed3b4-dc53-4ccd-91b7-93b67a0eba97" xmlns:ns3="63e8c1f7-1787-49b1-80e5-dcc3ae9ab6e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49dcd01241987285feedf33fb68cd0eb" ns2:_="" ns3:_="">
     <xsd:import namespace="977ed3b4-dc53-4ccd-91b7-93b67a0eba97"/>
@@ -12172,27 +12648,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1248F1AE-3111-486C-9539-89A3A0C8DC46}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="977ed3b4-dc53-4ccd-91b7-93b67a0eba97"/>
+    <ds:schemaRef ds:uri="63e8c1f7-1787-49b1-80e5-dcc3ae9ab6e9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="977ed3b4-dc53-4ccd-91b7-93b67a0eba97">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="63e8c1f7-1787-49b1-80e5-dcc3ae9ab6e9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76C9B0CF-B37D-416E-8DE0-1FCA3098CD48}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EA66D22-701A-4111-9554-D131D04520EA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12209,23 +12684,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76C9B0CF-B37D-416E-8DE0-1FCA3098CD48}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1248F1AE-3111-486C-9539-89A3A0C8DC46}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="977ed3b4-dc53-4ccd-91b7-93b67a0eba97"/>
-    <ds:schemaRef ds:uri="63e8c1f7-1787-49b1-80e5-dcc3ae9ab6e9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>